<commit_message>
Improved the .apsimx file to HTML export
</commit_message>
<xml_diff>
--- a/Tests/Wheat/Observed.xlsx
+++ b/Tests/Wheat/Observed.xlsx
@@ -25,12 +25,6 @@
     <t>Clock.Today</t>
   </si>
   <si>
-    <t>LAI</t>
-  </si>
-  <si>
-    <t>LAIerror</t>
-  </si>
-  <si>
     <t>Wheat.Zadok.Stage</t>
   </si>
   <si>
@@ -602,6 +596,12 @@
   </si>
   <si>
     <t>Mer73NRate15WaterDry</t>
+  </si>
+  <si>
+    <t>Wheat.Leaf.LAI</t>
+  </si>
+  <si>
+    <t>Wheat.Leaf.LAIerror</t>
   </si>
 </sst>
 </file>
@@ -950,10 +950,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="588" topLeftCell="A151" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <pane ySplit="588" activePane="bottomLeft"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -965,7 +965,7 @@
     <col min="5" max="5" width="34.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" customWidth="1"/>
     <col min="7" max="7" width="26.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="23.33203125" customWidth="1"/>
     <col min="11" max="11" width="27.6640625" customWidth="1"/>
@@ -996,93 +996,93 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="AB1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
@@ -1158,7 +1158,7 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1">
@@ -1196,7 +1196,7 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
@@ -1234,7 +1234,7 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
@@ -1272,7 +1272,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
@@ -1310,7 +1310,7 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -1348,7 +1348,7 @@
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
@@ -1386,7 +1386,7 @@
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
@@ -1424,7 +1424,7 @@
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
@@ -1462,7 +1462,7 @@
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
@@ -1500,7 +1500,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
@@ -1538,7 +1538,7 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
@@ -1576,7 +1576,7 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1">
@@ -1614,7 +1614,7 @@
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1">
@@ -1652,7 +1652,7 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
@@ -1690,7 +1690,7 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
@@ -1728,7 +1728,7 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
@@ -1766,7 +1766,7 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1">
@@ -1804,7 +1804,7 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
@@ -1842,7 +1842,7 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
@@ -1880,7 +1880,7 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1">
@@ -1918,7 +1918,7 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1">
@@ -1956,7 +1956,7 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1">
@@ -1994,7 +1994,7 @@
     </row>
     <row r="26" spans="1:30">
       <c r="A26" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1">
@@ -2042,7 +2042,7 @@
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1">
@@ -2090,7 +2090,7 @@
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1">
@@ -2138,7 +2138,7 @@
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1">
@@ -2186,7 +2186,7 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1">
@@ -2234,7 +2234,7 @@
     </row>
     <row r="31" spans="1:30">
       <c r="A31" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1">
@@ -2282,7 +2282,7 @@
     </row>
     <row r="32" spans="1:30">
       <c r="A32" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1">
@@ -2330,7 +2330,7 @@
     </row>
     <row r="33" spans="1:30">
       <c r="A33" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1">
@@ -2378,7 +2378,7 @@
     </row>
     <row r="34" spans="1:30">
       <c r="A34" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1">
@@ -2426,7 +2426,7 @@
     </row>
     <row r="35" spans="1:30">
       <c r="A35" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1">
@@ -2474,7 +2474,7 @@
     </row>
     <row r="36" spans="1:30">
       <c r="A36" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1">
@@ -2522,7 +2522,7 @@
     </row>
     <row r="37" spans="1:30">
       <c r="A37" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1">
@@ -2570,7 +2570,7 @@
     </row>
     <row r="38" spans="1:30">
       <c r="A38" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B38" s="2">
         <v>34912</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="39" spans="1:30">
       <c r="A39" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2">
         <v>34942</v>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="40" spans="1:30">
       <c r="A40" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2">
         <v>34962</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="41" spans="1:30">
       <c r="A41" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2">
         <v>34991</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="42" spans="1:30">
       <c r="A42" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2">
         <v>34912</v>
@@ -2798,7 +2798,7 @@
     </row>
     <row r="43" spans="1:30">
       <c r="A43" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B43" s="2">
         <v>34942</v>
@@ -2842,7 +2842,7 @@
     </row>
     <row r="44" spans="1:30">
       <c r="A44" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B44" s="2">
         <v>34962</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="45" spans="1:30">
       <c r="A45" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B45" s="2">
         <v>34991</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="46" spans="1:30">
       <c r="A46" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2">
         <v>34912</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="47" spans="1:30">
       <c r="A47" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" s="2">
         <v>34942</v>
@@ -3028,7 +3028,7 @@
     </row>
     <row r="48" spans="1:30">
       <c r="A48" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B48" s="2">
         <v>34962</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="49" spans="1:30">
       <c r="A49" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B49" s="2">
         <v>34991</v>
@@ -3126,7 +3126,7 @@
     </row>
     <row r="50" spans="1:30">
       <c r="A50" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B50" s="2">
         <v>34912</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="51" spans="1:30">
       <c r="A51" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B51" s="2">
         <v>34942</v>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="52" spans="1:30">
       <c r="A52" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B52" s="2">
         <v>34962</v>
@@ -3258,7 +3258,7 @@
     </row>
     <row r="53" spans="1:30">
       <c r="A53" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B53" s="2">
         <v>34991</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="54" spans="1:30">
       <c r="A54" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B54" s="2">
         <v>34912</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="55" spans="1:30">
       <c r="A55" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B55" s="2">
         <v>34942</v>
@@ -3400,7 +3400,7 @@
     </row>
     <row r="56" spans="1:30">
       <c r="A56" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B56" s="2">
         <v>34962</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="57" spans="1:30">
       <c r="A57" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B57" s="2">
         <v>34991</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="58" spans="1:30">
       <c r="A58" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B58" s="2">
         <v>34912</v>
@@ -3542,7 +3542,7 @@
     </row>
     <row r="59" spans="1:30">
       <c r="A59" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B59" s="2">
         <v>34942</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="60" spans="1:30">
       <c r="A60" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B60" s="2">
         <v>34962</v>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="61" spans="1:30">
       <c r="A61" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B61" s="2">
         <v>34991</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="62" spans="1:30">
       <c r="A62" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B62" s="2">
         <v>34912</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="63" spans="1:30">
       <c r="A63" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B63" s="2">
         <v>34942</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="64" spans="1:30">
       <c r="A64" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B64" s="2">
         <v>34962</v>
@@ -3816,7 +3816,7 @@
     </row>
     <row r="65" spans="1:30">
       <c r="A65" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B65" s="2">
         <v>34991</v>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="66" spans="1:30">
       <c r="A66" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B66" s="2">
         <v>34912</v>
@@ -3914,7 +3914,7 @@
     </row>
     <row r="67" spans="1:30">
       <c r="A67" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B67" s="2">
         <v>34942</v>
@@ -3958,7 +3958,7 @@
     </row>
     <row r="68" spans="1:30">
       <c r="A68" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B68" s="2">
         <v>34962</v>
@@ -4002,7 +4002,7 @@
     </row>
     <row r="69" spans="1:30">
       <c r="A69" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B69" s="2">
         <v>34991</v>
@@ -4056,7 +4056,7 @@
     </row>
     <row r="70" spans="1:30">
       <c r="A70" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B70" s="2">
         <v>33797</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="71" spans="1:30">
       <c r="A71" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B71" s="2">
         <v>33812</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="72" spans="1:30">
       <c r="A72" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B72" s="2">
         <v>33840</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="73" spans="1:30">
       <c r="A73" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B73" s="2">
         <v>33856</v>
@@ -4328,7 +4328,7 @@
     </row>
     <row r="74" spans="1:30">
       <c r="A74" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B74" s="2">
         <v>33877</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="75" spans="1:30">
       <c r="A75" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B75" s="2">
         <v>33889</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="76" spans="1:30">
       <c r="A76" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B76" s="2">
         <v>33907</v>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="77" spans="1:30">
       <c r="A77" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B77" s="2">
         <v>33797</v>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="78" spans="1:30">
       <c r="A78" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B78" s="2">
         <v>33812</v>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="79" spans="1:30">
       <c r="A79" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B79" s="2">
         <v>33840</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="80" spans="1:30">
       <c r="A80" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B80" s="2">
         <v>33856</v>
@@ -4804,7 +4804,7 @@
     </row>
     <row r="81" spans="1:30">
       <c r="A81" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B81" s="2">
         <v>33877</v>
@@ -4876,7 +4876,7 @@
     </row>
     <row r="82" spans="1:30">
       <c r="A82" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B82" s="2">
         <v>33889</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="83" spans="1:30">
       <c r="A83" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B83" s="2">
         <v>33907</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="84" spans="1:30">
       <c r="A84" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B84" s="2">
         <v>33797</v>
@@ -5072,7 +5072,7 @@
     </row>
     <row r="85" spans="1:30">
       <c r="A85" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B85" s="2">
         <v>33812</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="86" spans="1:30">
       <c r="A86" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B86" s="2">
         <v>33840</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="87" spans="1:30">
       <c r="A87" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B87" s="2">
         <v>33856</v>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="88" spans="1:30">
       <c r="A88" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B88" s="2">
         <v>33877</v>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="89" spans="1:30">
       <c r="A89" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B89" s="2">
         <v>33889</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="90" spans="1:30">
       <c r="A90" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B90" s="2">
         <v>33907</v>
@@ -5484,7 +5484,7 @@
     </row>
     <row r="91" spans="1:30">
       <c r="A91" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B91" s="2">
         <v>33797</v>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="92" spans="1:30">
       <c r="A92" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B92" s="2">
         <v>33812</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="93" spans="1:30">
       <c r="A93" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B93" s="2">
         <v>33840</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="94" spans="1:30">
       <c r="A94" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B94" s="2">
         <v>33856</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="95" spans="1:30">
       <c r="A95" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B95" s="2">
         <v>33877</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="96" spans="1:30">
       <c r="A96" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B96" s="2">
         <v>33889</v>
@@ -5904,7 +5904,7 @@
     </row>
     <row r="97" spans="1:30">
       <c r="A97" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B97" s="2">
         <v>33907</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="98" spans="1:30">
       <c r="A98" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B98" s="2">
         <v>33797</v>
@@ -6024,7 +6024,7 @@
     </row>
     <row r="99" spans="1:30">
       <c r="A99" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B99" s="2">
         <v>33812</v>
@@ -6088,7 +6088,7 @@
     </row>
     <row r="100" spans="1:30">
       <c r="A100" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B100" s="2">
         <v>33840</v>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="101" spans="1:30">
       <c r="A101" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B101" s="2">
         <v>33856</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="102" spans="1:30">
       <c r="A102" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B102" s="2">
         <v>33877</v>
@@ -6304,7 +6304,7 @@
     </row>
     <row r="103" spans="1:30">
       <c r="A103" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B103" s="2">
         <v>33889</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="104" spans="1:30">
       <c r="A104" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B104" s="2">
         <v>33907</v>
@@ -6424,7 +6424,7 @@
     </row>
     <row r="105" spans="1:30">
       <c r="A105" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B105" s="2">
         <v>33797</v>
@@ -6488,7 +6488,7 @@
     </row>
     <row r="106" spans="1:30">
       <c r="A106" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B106" s="2">
         <v>33812</v>
@@ -6552,7 +6552,7 @@
     </row>
     <row r="107" spans="1:30">
       <c r="A107" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B107" s="2">
         <v>33840</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="108" spans="1:30">
       <c r="A108" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B108" s="2">
         <v>33856</v>
@@ -6696,7 +6696,7 @@
     </row>
     <row r="109" spans="1:30">
       <c r="A109" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B109" s="2">
         <v>33877</v>
@@ -6768,7 +6768,7 @@
     </row>
     <row r="110" spans="1:30">
       <c r="A110" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B110" s="2">
         <v>33889</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="111" spans="1:30">
       <c r="A111" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B111" s="2">
         <v>33907</v>
@@ -6900,7 +6900,7 @@
     </row>
     <row r="112" spans="1:30">
       <c r="A112" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1">
@@ -6938,7 +6938,7 @@
     </row>
     <row r="113" spans="1:30">
       <c r="A113" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1">
@@ -6976,7 +6976,7 @@
     </row>
     <row r="114" spans="1:30">
       <c r="A114" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1">
@@ -7014,7 +7014,7 @@
     </row>
     <row r="115" spans="1:30">
       <c r="A115" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1">
@@ -7052,7 +7052,7 @@
     </row>
     <row r="116" spans="1:30">
       <c r="A116" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1">
@@ -7090,7 +7090,7 @@
     </row>
     <row r="117" spans="1:30">
       <c r="A117" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1">
@@ -7128,7 +7128,7 @@
     </row>
     <row r="118" spans="1:30">
       <c r="A118" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1">
@@ -7166,7 +7166,7 @@
     </row>
     <row r="119" spans="1:30">
       <c r="A119" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1">
@@ -7204,7 +7204,7 @@
     </row>
     <row r="120" spans="1:30">
       <c r="A120" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1">
@@ -7242,7 +7242,7 @@
     </row>
     <row r="121" spans="1:30">
       <c r="A121" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1">
@@ -7280,7 +7280,7 @@
     </row>
     <row r="122" spans="1:30">
       <c r="A122" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1">
@@ -7318,7 +7318,7 @@
     </row>
     <row r="123" spans="1:30">
       <c r="A123" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1">
@@ -7356,7 +7356,7 @@
     </row>
     <row r="124" spans="1:30">
       <c r="A124" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1">
@@ -7394,7 +7394,7 @@
     </row>
     <row r="125" spans="1:30">
       <c r="A125" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1">
@@ -7432,7 +7432,7 @@
     </row>
     <row r="126" spans="1:30">
       <c r="A126" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1">
@@ -7470,7 +7470,7 @@
     </row>
     <row r="127" spans="1:30">
       <c r="A127" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1">
@@ -7508,7 +7508,7 @@
     </row>
     <row r="128" spans="1:30">
       <c r="A128" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1">
@@ -7546,7 +7546,7 @@
     </row>
     <row r="129" spans="1:30">
       <c r="A129" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1">
@@ -7590,7 +7590,7 @@
     </row>
     <row r="130" spans="1:30">
       <c r="A130" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1">
@@ -7634,7 +7634,7 @@
     </row>
     <row r="131" spans="1:30">
       <c r="A131" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1">
@@ -7678,7 +7678,7 @@
     </row>
     <row r="132" spans="1:30">
       <c r="A132" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1">
@@ -7724,7 +7724,7 @@
     </row>
     <row r="133" spans="1:30">
       <c r="A133" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1">
@@ -7770,7 +7770,7 @@
     </row>
     <row r="134" spans="1:30">
       <c r="A134" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1">
@@ -7816,7 +7816,7 @@
     </row>
     <row r="135" spans="1:30">
       <c r="A135" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="1">
@@ -7862,7 +7862,7 @@
     </row>
     <row r="136" spans="1:30">
       <c r="A136" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1">
@@ -7908,7 +7908,7 @@
     </row>
     <row r="137" spans="1:30">
       <c r="A137" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1">
@@ -7952,7 +7952,7 @@
     </row>
     <row r="138" spans="1:30">
       <c r="A138" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1">
@@ -7996,7 +7996,7 @@
     </row>
     <row r="139" spans="1:30">
       <c r="A139" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1">
@@ -8040,7 +8040,7 @@
     </row>
     <row r="140" spans="1:30">
       <c r="A140" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1">
@@ -8084,7 +8084,7 @@
     </row>
     <row r="141" spans="1:30">
       <c r="A141" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1">
@@ -8128,7 +8128,7 @@
     </row>
     <row r="142" spans="1:30">
       <c r="A142" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1">
@@ -8172,7 +8172,7 @@
     </row>
     <row r="143" spans="1:30">
       <c r="A143" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1">
@@ -8216,7 +8216,7 @@
     </row>
     <row r="144" spans="1:30">
       <c r="A144" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1">
@@ -8260,7 +8260,7 @@
     </row>
     <row r="145" spans="1:30">
       <c r="A145" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1">
@@ -8304,7 +8304,7 @@
     </row>
     <row r="146" spans="1:30">
       <c r="A146" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1">
@@ -8348,7 +8348,7 @@
     </row>
     <row r="147" spans="1:30">
       <c r="A147" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1">
@@ -8392,7 +8392,7 @@
     </row>
     <row r="148" spans="1:30">
       <c r="A148" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1">
@@ -8436,7 +8436,7 @@
     </row>
     <row r="149" spans="1:30">
       <c r="A149" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1">
@@ -8480,7 +8480,7 @@
     </row>
     <row r="150" spans="1:30">
       <c r="A150" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1">
@@ -8524,7 +8524,7 @@
     </row>
     <row r="151" spans="1:30">
       <c r="A151" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1">
@@ -8568,7 +8568,7 @@
     </row>
     <row r="152" spans="1:30">
       <c r="A152" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1">
@@ -8612,7 +8612,7 @@
     </row>
     <row r="153" spans="1:30">
       <c r="A153" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1">
@@ -8664,7 +8664,7 @@
     </row>
     <row r="154" spans="1:30">
       <c r="A154" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1">
@@ -8716,7 +8716,7 @@
     </row>
     <row r="155" spans="1:30">
       <c r="A155" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1">
@@ -8770,7 +8770,7 @@
     </row>
     <row r="156" spans="1:30">
       <c r="A156" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B156" s="1"/>
       <c r="C156" s="1">
@@ -8824,7 +8824,7 @@
     </row>
     <row r="157" spans="1:30">
       <c r="A157" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B157" s="1"/>
       <c r="C157" s="1">
@@ -8878,7 +8878,7 @@
     </row>
     <row r="158" spans="1:30">
       <c r="A158" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1">
@@ -8922,7 +8922,7 @@
     </row>
     <row r="159" spans="1:30">
       <c r="A159" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1">
@@ -8966,7 +8966,7 @@
     </row>
     <row r="160" spans="1:30">
       <c r="A160" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1">
@@ -9010,7 +9010,7 @@
     </row>
     <row r="161" spans="1:30">
       <c r="A161" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B161" s="1"/>
       <c r="C161" s="1">
@@ -9054,7 +9054,7 @@
     </row>
     <row r="162" spans="1:30">
       <c r="A162" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1">
@@ -9098,7 +9098,7 @@
     </row>
     <row r="163" spans="1:30">
       <c r="A163" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B163" s="1"/>
       <c r="C163" s="1">
@@ -9142,7 +9142,7 @@
     </row>
     <row r="164" spans="1:30">
       <c r="A164" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1">
@@ -9194,7 +9194,7 @@
     </row>
     <row r="165" spans="1:30">
       <c r="A165" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B165" s="1"/>
       <c r="C165" s="1">
@@ -9246,7 +9246,7 @@
     </row>
     <row r="166" spans="1:30">
       <c r="A166" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B166" s="1"/>
       <c r="C166" s="1">
@@ -9298,7 +9298,7 @@
     </row>
     <row r="167" spans="1:30">
       <c r="A167" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1">
@@ -9350,7 +9350,7 @@
     </row>
     <row r="168" spans="1:30">
       <c r="A168" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B168" s="1"/>
       <c r="C168" s="1">
@@ -9402,7 +9402,7 @@
     </row>
     <row r="169" spans="1:30">
       <c r="A169" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B169" s="1"/>
       <c r="C169" s="1">
@@ -9454,7 +9454,7 @@
     </row>
     <row r="170" spans="1:30">
       <c r="A170" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B170" s="1"/>
       <c r="C170" s="1">
@@ -9506,7 +9506,7 @@
     </row>
     <row r="171" spans="1:30">
       <c r="A171" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B171" s="1"/>
       <c r="C171" s="1">
@@ -9558,7 +9558,7 @@
     </row>
     <row r="172" spans="1:30">
       <c r="A172" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B172" s="1"/>
       <c r="C172" s="1">
@@ -9610,7 +9610,7 @@
     </row>
     <row r="173" spans="1:30">
       <c r="A173" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B173" s="1"/>
       <c r="C173" s="1">
@@ -9662,7 +9662,7 @@
     </row>
     <row r="174" spans="1:30">
       <c r="A174" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B174" s="1"/>
       <c r="C174" s="1">
@@ -9714,7 +9714,7 @@
     </row>
     <row r="175" spans="1:30">
       <c r="A175" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B175" s="1"/>
       <c r="C175" s="1">
@@ -9766,7 +9766,7 @@
     </row>
     <row r="176" spans="1:30">
       <c r="A176" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B176" s="1"/>
       <c r="C176" s="1">
@@ -9818,7 +9818,7 @@
     </row>
     <row r="177" spans="1:30">
       <c r="A177" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B177" s="1"/>
       <c r="C177" s="1">
@@ -9870,7 +9870,7 @@
     </row>
     <row r="178" spans="1:30">
       <c r="A178" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B178" s="1"/>
       <c r="C178" s="1">
@@ -9922,7 +9922,7 @@
     </row>
     <row r="179" spans="1:30">
       <c r="A179" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B179" s="1"/>
       <c r="C179" s="1">
@@ -9974,7 +9974,7 @@
     </row>
     <row r="180" spans="1:30">
       <c r="A180" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B180" s="1"/>
       <c r="C180" s="1">
@@ -10026,7 +10026,7 @@
     </row>
     <row r="181" spans="1:30">
       <c r="A181" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1">
@@ -10078,7 +10078,7 @@
     </row>
     <row r="182" spans="1:30">
       <c r="A182" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B182" s="1"/>
       <c r="C182" s="1">
@@ -10130,7 +10130,7 @@
     </row>
     <row r="183" spans="1:30">
       <c r="A183" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B183" s="1"/>
       <c r="C183" s="1">
@@ -10182,7 +10182,7 @@
     </row>
     <row r="184" spans="1:30">
       <c r="A184" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B184" s="1"/>
       <c r="C184" s="1">
@@ -10234,7 +10234,7 @@
     </row>
     <row r="185" spans="1:30">
       <c r="A185" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B185" s="1"/>
       <c r="C185" s="1">
@@ -10286,7 +10286,7 @@
     </row>
     <row r="186" spans="1:30">
       <c r="A186" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B186" s="1"/>
       <c r="C186" s="1">
@@ -10338,7 +10338,7 @@
     </row>
     <row r="187" spans="1:30">
       <c r="A187" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B187" s="1"/>
       <c r="C187" s="1">
@@ -10390,7 +10390,7 @@
     </row>
     <row r="188" spans="1:30">
       <c r="A188" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1">
@@ -10442,7 +10442,7 @@
     </row>
     <row r="189" spans="1:30">
       <c r="A189" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B189" s="1"/>
       <c r="C189" s="1">
@@ -10494,7 +10494,7 @@
     </row>
     <row r="190" spans="1:30">
       <c r="A190" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B190" s="1"/>
       <c r="C190" s="1">
@@ -10546,7 +10546,7 @@
     </row>
     <row r="191" spans="1:30">
       <c r="A191" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B191" s="1"/>
       <c r="C191" s="1">
@@ -10598,7 +10598,7 @@
     </row>
     <row r="192" spans="1:30">
       <c r="A192" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B192" s="1"/>
       <c r="C192" s="1">
@@ -10650,7 +10650,7 @@
     </row>
     <row r="193" spans="1:30">
       <c r="A193" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B193" s="1"/>
       <c r="C193" s="1">
@@ -10702,7 +10702,7 @@
     </row>
     <row r="194" spans="1:30">
       <c r="A194" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="1">
@@ -10754,7 +10754,7 @@
     </row>
     <row r="195" spans="1:30">
       <c r="A195" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1">
@@ -10806,7 +10806,7 @@
     </row>
     <row r="196" spans="1:30">
       <c r="A196" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="1">
@@ -10858,7 +10858,7 @@
     </row>
     <row r="197" spans="1:30">
       <c r="A197" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B197" s="1"/>
       <c r="C197" s="1">
@@ -10900,7 +10900,7 @@
     </row>
     <row r="198" spans="1:30">
       <c r="A198" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1">
@@ -10954,7 +10954,7 @@
     </row>
     <row r="199" spans="1:30">
       <c r="A199" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1">
@@ -11008,7 +11008,7 @@
     </row>
     <row r="200" spans="1:30">
       <c r="A200" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1">
@@ -11062,7 +11062,7 @@
     </row>
     <row r="201" spans="1:30">
       <c r="A201" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1">
@@ -11116,7 +11116,7 @@
     </row>
     <row r="202" spans="1:30">
       <c r="A202" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1">
@@ -11170,7 +11170,7 @@
     </row>
     <row r="203" spans="1:30">
       <c r="A203" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1">
@@ -11224,7 +11224,7 @@
     </row>
     <row r="204" spans="1:30">
       <c r="A204" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1">
@@ -11278,7 +11278,7 @@
     </row>
     <row r="205" spans="1:30">
       <c r="A205" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1">
@@ -11324,7 +11324,7 @@
     </row>
     <row r="206" spans="1:30">
       <c r="A206" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1">
@@ -11370,7 +11370,7 @@
     </row>
     <row r="207" spans="1:30">
       <c r="A207" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1">
@@ -11424,7 +11424,7 @@
     </row>
     <row r="208" spans="1:30">
       <c r="A208" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1">
@@ -11474,7 +11474,7 @@
     </row>
     <row r="209" spans="1:30">
       <c r="A209" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1">
@@ -11518,7 +11518,7 @@
     </row>
     <row r="210" spans="1:30">
       <c r="A210" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1">
@@ -11570,7 +11570,7 @@
     </row>
     <row r="211" spans="1:30">
       <c r="A211" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1">
@@ -11622,7 +11622,7 @@
     </row>
     <row r="212" spans="1:30">
       <c r="A212" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1">
@@ -11674,7 +11674,7 @@
     </row>
     <row r="213" spans="1:30">
       <c r="A213" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1">
@@ -11726,7 +11726,7 @@
     </row>
     <row r="214" spans="1:30">
       <c r="A214" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B214" s="1"/>
       <c r="C214" s="1">
@@ -11778,7 +11778,7 @@
     </row>
     <row r="215" spans="1:30">
       <c r="A215" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1">
@@ -11830,7 +11830,7 @@
     </row>
     <row r="216" spans="1:30">
       <c r="A216" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1">
@@ -11882,7 +11882,7 @@
     </row>
     <row r="217" spans="1:30">
       <c r="A217" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1">
@@ -11934,7 +11934,7 @@
     </row>
     <row r="218" spans="1:30">
       <c r="A218" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1">
@@ -11986,7 +11986,7 @@
     </row>
     <row r="219" spans="1:30">
       <c r="A219" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1">
@@ -12038,7 +12038,7 @@
     </row>
     <row r="220" spans="1:30">
       <c r="A220" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B220" s="1"/>
       <c r="C220" s="1">
@@ -12088,7 +12088,7 @@
     </row>
     <row r="221" spans="1:30">
       <c r="A221" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1">
@@ -12138,7 +12138,7 @@
     </row>
     <row r="222" spans="1:30">
       <c r="A222" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B222" s="1"/>
       <c r="C222" s="1">
@@ -12188,7 +12188,7 @@
     </row>
     <row r="223" spans="1:30">
       <c r="A223" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B223" s="1"/>
       <c r="C223" s="1">
@@ -12238,7 +12238,7 @@
     </row>
     <row r="224" spans="1:30">
       <c r="A224" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1">
@@ -12278,7 +12278,7 @@
     </row>
     <row r="225" spans="1:30">
       <c r="A225" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B225" s="1"/>
       <c r="C225" s="1">
@@ -12318,7 +12318,7 @@
     </row>
     <row r="226" spans="1:30">
       <c r="A226" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B226" s="1"/>
       <c r="C226" s="1">

</xml_diff>

<commit_message>
update wheat validation to include cunderdin site
</commit_message>
<xml_diff>
--- a/Tests/Wheat/Observed.xlsx
+++ b/Tests/Wheat/Observed.xlsx
@@ -160,108 +160,6 @@
     <t>Nrate</t>
   </si>
   <si>
-    <t>Wheat_Cunderdin97_DryN0SpearEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN0SpearMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN50SpearEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN50SpearMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0SpearEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0SpearMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN50SpearEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN50SpearMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN0WilgoyneEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN0WilgoyneMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN0WilgoyneLate</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN50WilgoyneEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN50WilgoyneMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0WilgoyneEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0WilgoyneMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0WilgoyneLate</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN50WilgoyneEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN50WilgoyneMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN0bSpearEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN0bSpearMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN50bSpearEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN50bSpearMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0bSpearEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0bSpearMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN50bSpearEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN50bSpearMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN0bWilgoyneEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN0bWilgoyneMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN50bWilgoyneEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_DryN50bWilgoyneMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0bWilgoyneEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN0bWilgoyneMid</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN50bWilgoyneEarly</t>
-  </si>
-  <si>
-    <t>Wheat_Cunderdin97_WetN50bWilgoyneMid</t>
-  </si>
-  <si>
     <t>Wheat_Wongan84_N000</t>
   </si>
   <si>
@@ -602,6 +500,108 @@
   </si>
   <si>
     <t>Wheat.Leaf.LAIerror</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlySowN0TopN30IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearMidSowN0TopN30IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneEarlySowN0TopN30IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneMidSowN0TopN30IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlySowN0TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlyMidN0TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneEarlySowN0TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneLateSowN0TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneMidSowN0TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlySowN50TopN30IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearMidSowN50TopN30IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneEarlySowN50TopN30IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneMidSowN50TopN30IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlySowN50TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearMidSowN50TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneEarlySowN50TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneMidSowN50TopN0IrrDry</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlySowN0TopN30IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearMidSowN0TopN30IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneEarlySowN0TopN30IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneMidSowN0TopN30IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlySowN0TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearMidSowN0TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneEarlySowN0TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneLateSowN0TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneMidSowN0TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlySowN50TopN30IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearMidSowN50TopN30IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneEarlySowN50TopN30IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneMidSowN50TopN30IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearEarlySowN50TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowSpearMidSowN50TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneEarlySowN50TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>Cunderdin97SowWilgoyneMidSowN50TopN0IrrWet</t>
   </si>
 </sst>
 </file>
@@ -950,16 +950,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <pane ySplit="588" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="588" topLeftCell="A111" activePane="bottomLeft"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="51.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="47.21875" customWidth="1"/>
     <col min="3" max="3" width="21.109375" customWidth="1"/>
     <col min="4" max="4" width="28.5546875" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" customWidth="1"/>
@@ -1011,10 +1011,10 @@
         <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>19</v>
@@ -1074,7 +1074,7 @@
         <v>45</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>46</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="5" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="5" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
@@ -1158,7 +1158,7 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="5" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1">
@@ -1196,7 +1196,7 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="5" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
@@ -1234,7 +1234,7 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="5" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
@@ -1272,7 +1272,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="5" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
@@ -1310,7 +1310,7 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -1348,7 +1348,7 @@
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="5" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
@@ -1386,7 +1386,7 @@
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="5" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
@@ -1424,7 +1424,7 @@
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="5" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
@@ -1462,7 +1462,7 @@
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="5" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
@@ -1500,7 +1500,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="5" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
@@ -1538,7 +1538,7 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="5" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
@@ -1576,7 +1576,7 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="5" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1">
@@ -1614,7 +1614,7 @@
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="5" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1">
@@ -1652,7 +1652,7 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="5" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
@@ -1690,7 +1690,7 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
@@ -1728,7 +1728,7 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="5" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
@@ -1766,7 +1766,7 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="5" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1">
@@ -1804,7 +1804,7 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="5" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
@@ -1842,7 +1842,7 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="5" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
@@ -1880,7 +1880,7 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="5" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1">
@@ -1918,7 +1918,7 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="5" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1">
@@ -1956,7 +1956,7 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="5" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1">
@@ -4056,7 +4056,7 @@
     </row>
     <row r="70" spans="1:30">
       <c r="A70" s="5" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B70" s="2">
         <v>33797</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="71" spans="1:30">
       <c r="A71" s="5" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B71" s="2">
         <v>33812</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="72" spans="1:30">
       <c r="A72" s="5" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2">
         <v>33840</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="73" spans="1:30">
       <c r="A73" s="5" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B73" s="2">
         <v>33856</v>
@@ -4328,7 +4328,7 @@
     </row>
     <row r="74" spans="1:30">
       <c r="A74" s="5" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B74" s="2">
         <v>33877</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="75" spans="1:30">
       <c r="A75" s="5" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B75" s="2">
         <v>33889</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="76" spans="1:30">
       <c r="A76" s="5" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B76" s="2">
         <v>33907</v>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="77" spans="1:30">
       <c r="A77" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B77" s="2">
         <v>33797</v>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="78" spans="1:30">
       <c r="A78" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B78" s="2">
         <v>33812</v>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="79" spans="1:30">
       <c r="A79" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B79" s="2">
         <v>33840</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="80" spans="1:30">
       <c r="A80" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B80" s="2">
         <v>33856</v>
@@ -4804,7 +4804,7 @@
     </row>
     <row r="81" spans="1:30">
       <c r="A81" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B81" s="2">
         <v>33877</v>
@@ -4876,7 +4876,7 @@
     </row>
     <row r="82" spans="1:30">
       <c r="A82" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B82" s="2">
         <v>33889</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="83" spans="1:30">
       <c r="A83" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B83" s="2">
         <v>33907</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="84" spans="1:30">
       <c r="A84" s="5" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B84" s="2">
         <v>33797</v>
@@ -5072,7 +5072,7 @@
     </row>
     <row r="85" spans="1:30">
       <c r="A85" s="5" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B85" s="2">
         <v>33812</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="86" spans="1:30">
       <c r="A86" s="5" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B86" s="2">
         <v>33840</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="87" spans="1:30">
       <c r="A87" s="5" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B87" s="2">
         <v>33856</v>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="88" spans="1:30">
       <c r="A88" s="5" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B88" s="2">
         <v>33877</v>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="89" spans="1:30">
       <c r="A89" s="5" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B89" s="2">
         <v>33889</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="90" spans="1:30">
       <c r="A90" s="5" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B90" s="2">
         <v>33907</v>
@@ -5484,7 +5484,7 @@
     </row>
     <row r="91" spans="1:30">
       <c r="A91" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B91" s="2">
         <v>33797</v>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="92" spans="1:30">
       <c r="A92" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B92" s="2">
         <v>33812</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="93" spans="1:30">
       <c r="A93" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B93" s="2">
         <v>33840</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="94" spans="1:30">
       <c r="A94" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B94" s="2">
         <v>33856</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="95" spans="1:30">
       <c r="A95" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B95" s="2">
         <v>33877</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="96" spans="1:30">
       <c r="A96" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B96" s="2">
         <v>33889</v>
@@ -5904,7 +5904,7 @@
     </row>
     <row r="97" spans="1:30">
       <c r="A97" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B97" s="2">
         <v>33907</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="98" spans="1:30">
       <c r="A98" s="5" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B98" s="2">
         <v>33797</v>
@@ -6024,7 +6024,7 @@
     </row>
     <row r="99" spans="1:30">
       <c r="A99" s="5" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B99" s="2">
         <v>33812</v>
@@ -6088,7 +6088,7 @@
     </row>
     <row r="100" spans="1:30">
       <c r="A100" s="5" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B100" s="2">
         <v>33840</v>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="101" spans="1:30">
       <c r="A101" s="5" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B101" s="2">
         <v>33856</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="102" spans="1:30">
       <c r="A102" s="5" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B102" s="2">
         <v>33877</v>
@@ -6304,7 +6304,7 @@
     </row>
     <row r="103" spans="1:30">
       <c r="A103" s="5" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B103" s="2">
         <v>33889</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="104" spans="1:30">
       <c r="A104" s="5" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B104" s="2">
         <v>33907</v>
@@ -6424,7 +6424,7 @@
     </row>
     <row r="105" spans="1:30">
       <c r="A105" s="5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B105" s="2">
         <v>33797</v>
@@ -6488,7 +6488,7 @@
     </row>
     <row r="106" spans="1:30">
       <c r="A106" s="5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B106" s="2">
         <v>33812</v>
@@ -6552,7 +6552,7 @@
     </row>
     <row r="107" spans="1:30">
       <c r="A107" s="5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B107" s="2">
         <v>33840</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="108" spans="1:30">
       <c r="A108" s="5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B108" s="2">
         <v>33856</v>
@@ -6696,7 +6696,7 @@
     </row>
     <row r="109" spans="1:30">
       <c r="A109" s="5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B109" s="2">
         <v>33877</v>
@@ -6768,7 +6768,7 @@
     </row>
     <row r="110" spans="1:30">
       <c r="A110" s="5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B110" s="2">
         <v>33889</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="111" spans="1:30">
       <c r="A111" s="5" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B111" s="2">
         <v>33907</v>
@@ -6900,7 +6900,7 @@
     </row>
     <row r="112" spans="1:30">
       <c r="A112" s="5" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1">
@@ -6938,7 +6938,7 @@
     </row>
     <row r="113" spans="1:30">
       <c r="A113" s="5" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1">
@@ -6976,7 +6976,7 @@
     </row>
     <row r="114" spans="1:30">
       <c r="A114" s="5" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1">
@@ -7014,7 +7014,7 @@
     </row>
     <row r="115" spans="1:30">
       <c r="A115" s="5" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1">
@@ -7052,7 +7052,7 @@
     </row>
     <row r="116" spans="1:30">
       <c r="A116" s="5" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1">
@@ -7090,7 +7090,7 @@
     </row>
     <row r="117" spans="1:30">
       <c r="A117" s="5" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1">
@@ -7128,7 +7128,7 @@
     </row>
     <row r="118" spans="1:30">
       <c r="A118" s="5" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1">
@@ -7166,7 +7166,7 @@
     </row>
     <row r="119" spans="1:30">
       <c r="A119" s="5" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1">
@@ -7204,7 +7204,7 @@
     </row>
     <row r="120" spans="1:30">
       <c r="A120" s="5" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1">
@@ -7242,7 +7242,7 @@
     </row>
     <row r="121" spans="1:30">
       <c r="A121" s="5" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1">
@@ -7280,7 +7280,7 @@
     </row>
     <row r="122" spans="1:30">
       <c r="A122" s="5" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1">
@@ -7318,7 +7318,7 @@
     </row>
     <row r="123" spans="1:30">
       <c r="A123" s="5" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1">
@@ -7356,7 +7356,7 @@
     </row>
     <row r="124" spans="1:30">
       <c r="A124" s="5" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1">
@@ -7394,7 +7394,7 @@
     </row>
     <row r="125" spans="1:30">
       <c r="A125" s="5" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1">
@@ -7432,7 +7432,7 @@
     </row>
     <row r="126" spans="1:30">
       <c r="A126" s="5" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1">
@@ -7470,7 +7470,7 @@
     </row>
     <row r="127" spans="1:30">
       <c r="A127" s="5" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1">
@@ -7508,7 +7508,7 @@
     </row>
     <row r="128" spans="1:30">
       <c r="A128" s="5" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1">
@@ -7546,7 +7546,7 @@
     </row>
     <row r="129" spans="1:30">
       <c r="A129" s="5" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1">
@@ -7590,7 +7590,7 @@
     </row>
     <row r="130" spans="1:30">
       <c r="A130" s="5" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1">
@@ -7634,7 +7634,7 @@
     </row>
     <row r="131" spans="1:30">
       <c r="A131" s="5" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1">
@@ -7678,7 +7678,7 @@
     </row>
     <row r="132" spans="1:30">
       <c r="A132" s="5" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1">
@@ -7724,7 +7724,7 @@
     </row>
     <row r="133" spans="1:30">
       <c r="A133" s="5" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1">
@@ -7770,7 +7770,7 @@
     </row>
     <row r="134" spans="1:30">
       <c r="A134" s="5" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1">
@@ -7816,7 +7816,7 @@
     </row>
     <row r="135" spans="1:30">
       <c r="A135" s="5" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="1">
@@ -7862,7 +7862,7 @@
     </row>
     <row r="136" spans="1:30">
       <c r="A136" s="5" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1">
@@ -7908,7 +7908,7 @@
     </row>
     <row r="137" spans="1:30">
       <c r="A137" s="5" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1">
@@ -7952,7 +7952,7 @@
     </row>
     <row r="138" spans="1:30">
       <c r="A138" s="5" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1">
@@ -7996,7 +7996,7 @@
     </row>
     <row r="139" spans="1:30">
       <c r="A139" s="5" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1">
@@ -8040,7 +8040,7 @@
     </row>
     <row r="140" spans="1:30">
       <c r="A140" s="5" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1">
@@ -8084,7 +8084,7 @@
     </row>
     <row r="141" spans="1:30">
       <c r="A141" s="5" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1">
@@ -8128,7 +8128,7 @@
     </row>
     <row r="142" spans="1:30">
       <c r="A142" s="5" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1">
@@ -8172,7 +8172,7 @@
     </row>
     <row r="143" spans="1:30">
       <c r="A143" s="5" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1">
@@ -8216,7 +8216,7 @@
     </row>
     <row r="144" spans="1:30">
       <c r="A144" s="5" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1">
@@ -8260,7 +8260,7 @@
     </row>
     <row r="145" spans="1:30">
       <c r="A145" s="5" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1">
@@ -8304,7 +8304,7 @@
     </row>
     <row r="146" spans="1:30">
       <c r="A146" s="5" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1">
@@ -8348,7 +8348,7 @@
     </row>
     <row r="147" spans="1:30">
       <c r="A147" s="5" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1">
@@ -8392,7 +8392,7 @@
     </row>
     <row r="148" spans="1:30">
       <c r="A148" s="5" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1">
@@ -8436,7 +8436,7 @@
     </row>
     <row r="149" spans="1:30">
       <c r="A149" s="5" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1">
@@ -8480,7 +8480,7 @@
     </row>
     <row r="150" spans="1:30">
       <c r="A150" s="5" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1">
@@ -8524,7 +8524,7 @@
     </row>
     <row r="151" spans="1:30">
       <c r="A151" s="5" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1">
@@ -8568,7 +8568,7 @@
     </row>
     <row r="152" spans="1:30">
       <c r="A152" s="5" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1">
@@ -8612,7 +8612,7 @@
     </row>
     <row r="153" spans="1:30">
       <c r="A153" s="5" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1">
@@ -8664,7 +8664,7 @@
     </row>
     <row r="154" spans="1:30">
       <c r="A154" s="5" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1">
@@ -8716,7 +8716,7 @@
     </row>
     <row r="155" spans="1:30">
       <c r="A155" s="5" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1">
@@ -8770,7 +8770,7 @@
     </row>
     <row r="156" spans="1:30">
       <c r="A156" s="5" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B156" s="1"/>
       <c r="C156" s="1">
@@ -8824,7 +8824,7 @@
     </row>
     <row r="157" spans="1:30">
       <c r="A157" s="5" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="B157" s="1"/>
       <c r="C157" s="1">
@@ -8878,7 +8878,7 @@
     </row>
     <row r="158" spans="1:30">
       <c r="A158" s="5" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1">
@@ -8922,7 +8922,7 @@
     </row>
     <row r="159" spans="1:30">
       <c r="A159" s="5" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1">
@@ -8966,7 +8966,7 @@
     </row>
     <row r="160" spans="1:30">
       <c r="A160" s="5" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1">
@@ -9010,7 +9010,7 @@
     </row>
     <row r="161" spans="1:30">
       <c r="A161" s="5" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="B161" s="1"/>
       <c r="C161" s="1">
@@ -9054,7 +9054,7 @@
     </row>
     <row r="162" spans="1:30">
       <c r="A162" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1">
@@ -9098,7 +9098,7 @@
     </row>
     <row r="163" spans="1:30">
       <c r="A163" s="5" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="B163" s="1"/>
       <c r="C163" s="1">
@@ -9142,7 +9142,7 @@
     </row>
     <row r="164" spans="1:30">
       <c r="A164" s="5" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1">
@@ -9194,9 +9194,9 @@
     </row>
     <row r="165" spans="1:30">
       <c r="A165" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B165" s="1"/>
+        <v>162</v>
+      </c>
+      <c r="B165" s="5"/>
       <c r="C165" s="1">
         <v>90</v>
       </c>
@@ -9246,9 +9246,9 @@
     </row>
     <row r="166" spans="1:30">
       <c r="A166" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B166" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="B166" s="5"/>
       <c r="C166" s="1">
         <v>90</v>
       </c>
@@ -9298,9 +9298,9 @@
     </row>
     <row r="167" spans="1:30">
       <c r="A167" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B167" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="B167" s="5"/>
       <c r="C167" s="1">
         <v>90</v>
       </c>
@@ -9350,9 +9350,9 @@
     </row>
     <row r="168" spans="1:30">
       <c r="A168" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B168" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="B168" s="5"/>
       <c r="C168" s="1">
         <v>90</v>
       </c>
@@ -9402,9 +9402,9 @@
     </row>
     <row r="169" spans="1:30">
       <c r="A169" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B169" s="1"/>
+        <v>166</v>
+      </c>
+      <c r="B169" s="5"/>
       <c r="C169" s="1">
         <v>90</v>
       </c>
@@ -9454,9 +9454,9 @@
     </row>
     <row r="170" spans="1:30">
       <c r="A170" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B170" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="B170" s="5"/>
       <c r="C170" s="1">
         <v>90</v>
       </c>
@@ -9506,9 +9506,9 @@
     </row>
     <row r="171" spans="1:30">
       <c r="A171" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B171" s="1"/>
+        <v>168</v>
+      </c>
+      <c r="B171" s="5"/>
       <c r="C171" s="1">
         <v>90</v>
       </c>
@@ -9558,9 +9558,9 @@
     </row>
     <row r="172" spans="1:30">
       <c r="A172" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B172" s="1"/>
+        <v>169</v>
+      </c>
+      <c r="B172" s="5"/>
       <c r="C172" s="1">
         <v>90</v>
       </c>
@@ -9610,9 +9610,9 @@
     </row>
     <row r="173" spans="1:30">
       <c r="A173" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B173" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="B173" s="5"/>
       <c r="C173" s="1">
         <v>90</v>
       </c>
@@ -9662,9 +9662,9 @@
     </row>
     <row r="174" spans="1:30">
       <c r="A174" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B174" s="1"/>
+        <v>171</v>
+      </c>
+      <c r="B174" s="5"/>
       <c r="C174" s="1">
         <v>90</v>
       </c>
@@ -9714,9 +9714,9 @@
     </row>
     <row r="175" spans="1:30">
       <c r="A175" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B175" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="B175" s="5"/>
       <c r="C175" s="1">
         <v>90</v>
       </c>
@@ -9766,9 +9766,9 @@
     </row>
     <row r="176" spans="1:30">
       <c r="A176" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B176" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="B176" s="5"/>
       <c r="C176" s="1">
         <v>90</v>
       </c>
@@ -9818,9 +9818,9 @@
     </row>
     <row r="177" spans="1:30">
       <c r="A177" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B177" s="1"/>
+        <v>174</v>
+      </c>
+      <c r="B177" s="5"/>
       <c r="C177" s="1">
         <v>90</v>
       </c>
@@ -9870,9 +9870,9 @@
     </row>
     <row r="178" spans="1:30">
       <c r="A178" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B178" s="1"/>
+        <v>175</v>
+      </c>
+      <c r="B178" s="5"/>
       <c r="C178" s="1">
         <v>90</v>
       </c>
@@ -9922,9 +9922,9 @@
     </row>
     <row r="179" spans="1:30">
       <c r="A179" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B179" s="1"/>
+        <v>176</v>
+      </c>
+      <c r="B179" s="5"/>
       <c r="C179" s="1">
         <v>90</v>
       </c>
@@ -9974,9 +9974,9 @@
     </row>
     <row r="180" spans="1:30">
       <c r="A180" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B180" s="1"/>
+        <v>177</v>
+      </c>
+      <c r="B180" s="5"/>
       <c r="C180" s="1">
         <v>90</v>
       </c>
@@ -10026,9 +10026,9 @@
     </row>
     <row r="181" spans="1:30">
       <c r="A181" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B181" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="B181" s="5"/>
       <c r="C181" s="1">
         <v>90</v>
       </c>
@@ -10078,9 +10078,9 @@
     </row>
     <row r="182" spans="1:30">
       <c r="A182" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B182" s="1"/>
+        <v>179</v>
+      </c>
+      <c r="B182" s="5"/>
       <c r="C182" s="1">
         <v>90</v>
       </c>
@@ -10130,9 +10130,9 @@
     </row>
     <row r="183" spans="1:30">
       <c r="A183" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B183" s="1"/>
+        <v>180</v>
+      </c>
+      <c r="B183" s="5"/>
       <c r="C183" s="1">
         <v>90</v>
       </c>
@@ -10182,9 +10182,9 @@
     </row>
     <row r="184" spans="1:30">
       <c r="A184" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B184" s="1"/>
+        <v>181</v>
+      </c>
+      <c r="B184" s="5"/>
       <c r="C184" s="1">
         <v>90</v>
       </c>
@@ -10234,9 +10234,9 @@
     </row>
     <row r="185" spans="1:30">
       <c r="A185" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B185" s="1"/>
+        <v>182</v>
+      </c>
+      <c r="B185" s="5"/>
       <c r="C185" s="1">
         <v>90</v>
       </c>
@@ -10286,9 +10286,9 @@
     </row>
     <row r="186" spans="1:30">
       <c r="A186" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B186" s="1"/>
+        <v>183</v>
+      </c>
+      <c r="B186" s="5"/>
       <c r="C186" s="1">
         <v>90</v>
       </c>
@@ -10338,9 +10338,9 @@
     </row>
     <row r="187" spans="1:30">
       <c r="A187" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B187" s="1"/>
+        <v>184</v>
+      </c>
+      <c r="B187" s="5"/>
       <c r="C187" s="1">
         <v>90</v>
       </c>
@@ -10390,9 +10390,9 @@
     </row>
     <row r="188" spans="1:30">
       <c r="A188" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B188" s="1"/>
+        <v>185</v>
+      </c>
+      <c r="B188" s="5"/>
       <c r="C188" s="1">
         <v>90</v>
       </c>
@@ -10442,9 +10442,9 @@
     </row>
     <row r="189" spans="1:30">
       <c r="A189" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B189" s="1"/>
+        <v>186</v>
+      </c>
+      <c r="B189" s="5"/>
       <c r="C189" s="1">
         <v>90</v>
       </c>
@@ -10494,9 +10494,9 @@
     </row>
     <row r="190" spans="1:30">
       <c r="A190" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B190" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="B190" s="5"/>
       <c r="C190" s="1">
         <v>90</v>
       </c>
@@ -10546,9 +10546,9 @@
     </row>
     <row r="191" spans="1:30">
       <c r="A191" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B191" s="1"/>
+        <v>188</v>
+      </c>
+      <c r="B191" s="5"/>
       <c r="C191" s="1">
         <v>90</v>
       </c>
@@ -10598,9 +10598,9 @@
     </row>
     <row r="192" spans="1:30">
       <c r="A192" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B192" s="1"/>
+        <v>189</v>
+      </c>
+      <c r="B192" s="5"/>
       <c r="C192" s="1">
         <v>90</v>
       </c>
@@ -10650,9 +10650,9 @@
     </row>
     <row r="193" spans="1:30">
       <c r="A193" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B193" s="1"/>
+        <v>190</v>
+      </c>
+      <c r="B193" s="5"/>
       <c r="C193" s="1">
         <v>90</v>
       </c>
@@ -10702,9 +10702,9 @@
     </row>
     <row r="194" spans="1:30">
       <c r="A194" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B194" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="B194" s="5"/>
       <c r="C194" s="1">
         <v>90</v>
       </c>
@@ -10754,9 +10754,9 @@
     </row>
     <row r="195" spans="1:30">
       <c r="A195" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B195" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="B195" s="5"/>
       <c r="C195" s="1">
         <v>90</v>
       </c>
@@ -10806,9 +10806,9 @@
     </row>
     <row r="196" spans="1:30">
       <c r="A196" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B196" s="1"/>
+        <v>193</v>
+      </c>
+      <c r="B196" s="5"/>
       <c r="C196" s="1">
         <v>90</v>
       </c>
@@ -10858,9 +10858,9 @@
     </row>
     <row r="197" spans="1:30">
       <c r="A197" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B197" s="1"/>
+        <v>194</v>
+      </c>
+      <c r="B197" s="5"/>
       <c r="C197" s="1">
         <v>90</v>
       </c>
@@ -10900,7 +10900,7 @@
     </row>
     <row r="198" spans="1:30">
       <c r="A198" s="5" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1">
@@ -10954,7 +10954,7 @@
     </row>
     <row r="199" spans="1:30">
       <c r="A199" s="5" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1">
@@ -11008,7 +11008,7 @@
     </row>
     <row r="200" spans="1:30">
       <c r="A200" s="5" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1">
@@ -11062,7 +11062,7 @@
     </row>
     <row r="201" spans="1:30">
       <c r="A201" s="5" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1">
@@ -11116,7 +11116,7 @@
     </row>
     <row r="202" spans="1:30">
       <c r="A202" s="5" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1">
@@ -11170,7 +11170,7 @@
     </row>
     <row r="203" spans="1:30">
       <c r="A203" s="5" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1">
@@ -11224,7 +11224,7 @@
     </row>
     <row r="204" spans="1:30">
       <c r="A204" s="5" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1">
@@ -11278,7 +11278,7 @@
     </row>
     <row r="205" spans="1:30">
       <c r="A205" s="5" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1">
@@ -11324,7 +11324,7 @@
     </row>
     <row r="206" spans="1:30">
       <c r="A206" s="5" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1">
@@ -11370,7 +11370,7 @@
     </row>
     <row r="207" spans="1:30">
       <c r="A207" s="5" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1">
@@ -11424,7 +11424,7 @@
     </row>
     <row r="208" spans="1:30">
       <c r="A208" s="5" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1">
@@ -11474,7 +11474,7 @@
     </row>
     <row r="209" spans="1:30">
       <c r="A209" s="5" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1">
@@ -11518,7 +11518,7 @@
     </row>
     <row r="210" spans="1:30">
       <c r="A210" s="5" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1">
@@ -11570,7 +11570,7 @@
     </row>
     <row r="211" spans="1:30">
       <c r="A211" s="5" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1">
@@ -11622,7 +11622,7 @@
     </row>
     <row r="212" spans="1:30">
       <c r="A212" s="5" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1">
@@ -11674,7 +11674,7 @@
     </row>
     <row r="213" spans="1:30">
       <c r="A213" s="5" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1">
@@ -11726,7 +11726,7 @@
     </row>
     <row r="214" spans="1:30">
       <c r="A214" s="5" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B214" s="1"/>
       <c r="C214" s="1">
@@ -11778,7 +11778,7 @@
     </row>
     <row r="215" spans="1:30">
       <c r="A215" s="5" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1">
@@ -11830,7 +11830,7 @@
     </row>
     <row r="216" spans="1:30">
       <c r="A216" s="5" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1">
@@ -11882,7 +11882,7 @@
     </row>
     <row r="217" spans="1:30">
       <c r="A217" s="5" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1">
@@ -11934,7 +11934,7 @@
     </row>
     <row r="218" spans="1:30">
       <c r="A218" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1">
@@ -11986,7 +11986,7 @@
     </row>
     <row r="219" spans="1:30">
       <c r="A219" s="5" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1">
@@ -12038,7 +12038,7 @@
     </row>
     <row r="220" spans="1:30">
       <c r="A220" s="5" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="B220" s="1"/>
       <c r="C220" s="1">
@@ -12088,7 +12088,7 @@
     </row>
     <row r="221" spans="1:30">
       <c r="A221" s="5" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1">
@@ -12138,7 +12138,7 @@
     </row>
     <row r="222" spans="1:30">
       <c r="A222" s="5" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="B222" s="1"/>
       <c r="C222" s="1">
@@ -12188,7 +12188,7 @@
     </row>
     <row r="223" spans="1:30">
       <c r="A223" s="5" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="B223" s="1"/>
       <c r="C223" s="1">
@@ -12238,7 +12238,7 @@
     </row>
     <row r="224" spans="1:30">
       <c r="A224" s="5" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1">
@@ -12278,7 +12278,7 @@
     </row>
     <row r="225" spans="1:30">
       <c r="A225" s="5" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="B225" s="1"/>
       <c r="C225" s="1">
@@ -12318,7 +12318,7 @@
     </row>
     <row r="226" spans="1:30">
       <c r="A226" s="5" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="B226" s="1"/>
       <c r="C226" s="1">

</xml_diff>

<commit_message>
update wheat validation to include mouse site
</commit_message>
<xml_diff>
--- a/Tests/Wheat/Observed.xlsx
+++ b/Tests/Wheat/Observed.xlsx
@@ -379,57 +379,6 @@
     <t>Yucheng04</t>
   </si>
   <si>
-    <t>DamageControl</t>
-  </si>
-  <si>
-    <t>DamageEmerg05</t>
-  </si>
-  <si>
-    <t>DamageEmerg10</t>
-  </si>
-  <si>
-    <t>DamageEmerg25</t>
-  </si>
-  <si>
-    <t>DamageEmerg50</t>
-  </si>
-  <si>
-    <t>DamageTiller05</t>
-  </si>
-  <si>
-    <t>DamageTiller10</t>
-  </si>
-  <si>
-    <t>DamageTiller25</t>
-  </si>
-  <si>
-    <t>DamageTiller50</t>
-  </si>
-  <si>
-    <t>DamageBoot05</t>
-  </si>
-  <si>
-    <t>DamageBoot10</t>
-  </si>
-  <si>
-    <t>DamageBoot25</t>
-  </si>
-  <si>
-    <t>DamageBoot50</t>
-  </si>
-  <si>
-    <t>DamagePreHarv05</t>
-  </si>
-  <si>
-    <t>DamagePreHarv10</t>
-  </si>
-  <si>
-    <t>DamagePreHarv25</t>
-  </si>
-  <si>
-    <t>DamagePreHarv50</t>
-  </si>
-  <si>
     <t>Wheat.Grain.Protein</t>
   </si>
   <si>
@@ -602,6 +551,57 @@
   </si>
   <si>
     <t>Cunderdin97SowWilgoyneMidSowN50TopN0IrrWet</t>
+  </si>
+  <si>
+    <t>mouseDamageBoot05</t>
+  </si>
+  <si>
+    <t>mouseDamageBoot10</t>
+  </si>
+  <si>
+    <t>mouseDamageBoot25</t>
+  </si>
+  <si>
+    <t>mouseDamageBoot50</t>
+  </si>
+  <si>
+    <t>mouseDamageControl</t>
+  </si>
+  <si>
+    <t>mouseDamageEmerg05</t>
+  </si>
+  <si>
+    <t>mouseDamageEmerg10</t>
+  </si>
+  <si>
+    <t>mouseDamageEmerg25</t>
+  </si>
+  <si>
+    <t>mouseDamageEmerg50</t>
+  </si>
+  <si>
+    <t>mouseDamagePreHarv05</t>
+  </si>
+  <si>
+    <t>mouseDamagePreHarv10</t>
+  </si>
+  <si>
+    <t>mouseDamagePreHarv25</t>
+  </si>
+  <si>
+    <t>mouseDamagePreHarv50</t>
+  </si>
+  <si>
+    <t>mouseDamageTiller05</t>
+  </si>
+  <si>
+    <t>mouseDamageTiller10</t>
+  </si>
+  <si>
+    <t>mouseDamageTiller25</t>
+  </si>
+  <si>
+    <t>mouseDamageTiller50</t>
   </si>
 </sst>
 </file>
@@ -953,7 +953,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="588" topLeftCell="A111" activePane="bottomLeft"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
+      <selection pane="bottomLeft" activeCell="B112" sqref="B112:B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1011,10 +1011,10 @@
         <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>19</v>
@@ -1074,7 +1074,7 @@
         <v>45</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>46</v>
@@ -4056,7 +4056,7 @@
     </row>
     <row r="70" spans="1:30">
       <c r="A70" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B70" s="2">
         <v>33797</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="71" spans="1:30">
       <c r="A71" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B71" s="2">
         <v>33812</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="72" spans="1:30">
       <c r="A72" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B72" s="2">
         <v>33840</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="73" spans="1:30">
       <c r="A73" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B73" s="2">
         <v>33856</v>
@@ -4328,7 +4328,7 @@
     </row>
     <row r="74" spans="1:30">
       <c r="A74" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B74" s="2">
         <v>33877</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="75" spans="1:30">
       <c r="A75" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B75" s="2">
         <v>33889</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="76" spans="1:30">
       <c r="A76" s="5" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B76" s="2">
         <v>33907</v>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="77" spans="1:30">
       <c r="A77" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B77" s="2">
         <v>33797</v>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="78" spans="1:30">
       <c r="A78" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B78" s="2">
         <v>33812</v>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="79" spans="1:30">
       <c r="A79" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B79" s="2">
         <v>33840</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="80" spans="1:30">
       <c r="A80" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B80" s="2">
         <v>33856</v>
@@ -4804,7 +4804,7 @@
     </row>
     <row r="81" spans="1:30">
       <c r="A81" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B81" s="2">
         <v>33877</v>
@@ -4876,7 +4876,7 @@
     </row>
     <row r="82" spans="1:30">
       <c r="A82" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B82" s="2">
         <v>33889</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="83" spans="1:30">
       <c r="A83" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B83" s="2">
         <v>33907</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="84" spans="1:30">
       <c r="A84" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B84" s="2">
         <v>33797</v>
@@ -5072,7 +5072,7 @@
     </row>
     <row r="85" spans="1:30">
       <c r="A85" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B85" s="2">
         <v>33812</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="86" spans="1:30">
       <c r="A86" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B86" s="2">
         <v>33840</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="87" spans="1:30">
       <c r="A87" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B87" s="2">
         <v>33856</v>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="88" spans="1:30">
       <c r="A88" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B88" s="2">
         <v>33877</v>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="89" spans="1:30">
       <c r="A89" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B89" s="2">
         <v>33889</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="90" spans="1:30">
       <c r="A90" s="5" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="B90" s="2">
         <v>33907</v>
@@ -5484,7 +5484,7 @@
     </row>
     <row r="91" spans="1:30">
       <c r="A91" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B91" s="2">
         <v>33797</v>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="92" spans="1:30">
       <c r="A92" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B92" s="2">
         <v>33812</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="93" spans="1:30">
       <c r="A93" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B93" s="2">
         <v>33840</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="94" spans="1:30">
       <c r="A94" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B94" s="2">
         <v>33856</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="95" spans="1:30">
       <c r="A95" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B95" s="2">
         <v>33877</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="96" spans="1:30">
       <c r="A96" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B96" s="2">
         <v>33889</v>
@@ -5904,7 +5904,7 @@
     </row>
     <row r="97" spans="1:30">
       <c r="A97" s="5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B97" s="2">
         <v>33907</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="98" spans="1:30">
       <c r="A98" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B98" s="2">
         <v>33797</v>
@@ -6024,7 +6024,7 @@
     </row>
     <row r="99" spans="1:30">
       <c r="A99" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B99" s="2">
         <v>33812</v>
@@ -6088,7 +6088,7 @@
     </row>
     <row r="100" spans="1:30">
       <c r="A100" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B100" s="2">
         <v>33840</v>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="101" spans="1:30">
       <c r="A101" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B101" s="2">
         <v>33856</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="102" spans="1:30">
       <c r="A102" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B102" s="2">
         <v>33877</v>
@@ -6304,7 +6304,7 @@
     </row>
     <row r="103" spans="1:30">
       <c r="A103" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B103" s="2">
         <v>33889</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="104" spans="1:30">
       <c r="A104" s="5" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B104" s="2">
         <v>33907</v>
@@ -6424,7 +6424,7 @@
     </row>
     <row r="105" spans="1:30">
       <c r="A105" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B105" s="2">
         <v>33797</v>
@@ -6488,7 +6488,7 @@
     </row>
     <row r="106" spans="1:30">
       <c r="A106" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B106" s="2">
         <v>33812</v>
@@ -6552,7 +6552,7 @@
     </row>
     <row r="107" spans="1:30">
       <c r="A107" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B107" s="2">
         <v>33840</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="108" spans="1:30">
       <c r="A108" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B108" s="2">
         <v>33856</v>
@@ -6696,7 +6696,7 @@
     </row>
     <row r="109" spans="1:30">
       <c r="A109" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B109" s="2">
         <v>33877</v>
@@ -6768,7 +6768,7 @@
     </row>
     <row r="110" spans="1:30">
       <c r="A110" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B110" s="2">
         <v>33889</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="111" spans="1:30">
       <c r="A111" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B111" s="2">
         <v>33907</v>
@@ -6900,7 +6900,7 @@
     </row>
     <row r="112" spans="1:30">
       <c r="A112" s="5" t="s">
-        <v>129</v>
+        <v>178</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1">
@@ -6938,7 +6938,7 @@
     </row>
     <row r="113" spans="1:30">
       <c r="A113" s="5" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1">
@@ -6976,7 +6976,7 @@
     </row>
     <row r="114" spans="1:30">
       <c r="A114" s="5" t="s">
-        <v>131</v>
+        <v>180</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1">
@@ -7014,7 +7014,7 @@
     </row>
     <row r="115" spans="1:30">
       <c r="A115" s="5" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1">
@@ -7052,7 +7052,7 @@
     </row>
     <row r="116" spans="1:30">
       <c r="A116" s="5" t="s">
-        <v>120</v>
+        <v>182</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1">
@@ -7090,7 +7090,7 @@
     </row>
     <row r="117" spans="1:30">
       <c r="A117" s="5" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1">
@@ -7128,7 +7128,7 @@
     </row>
     <row r="118" spans="1:30">
       <c r="A118" s="5" t="s">
-        <v>122</v>
+        <v>184</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1">
@@ -7166,7 +7166,7 @@
     </row>
     <row r="119" spans="1:30">
       <c r="A119" s="5" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1">
@@ -7204,7 +7204,7 @@
     </row>
     <row r="120" spans="1:30">
       <c r="A120" s="5" t="s">
-        <v>124</v>
+        <v>186</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1">
@@ -7242,7 +7242,7 @@
     </row>
     <row r="121" spans="1:30">
       <c r="A121" s="5" t="s">
-        <v>133</v>
+        <v>187</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1">
@@ -7280,7 +7280,7 @@
     </row>
     <row r="122" spans="1:30">
       <c r="A122" s="5" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1">
@@ -7318,7 +7318,7 @@
     </row>
     <row r="123" spans="1:30">
       <c r="A123" s="5" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1">
@@ -7356,7 +7356,7 @@
     </row>
     <row r="124" spans="1:30">
       <c r="A124" s="5" t="s">
-        <v>136</v>
+        <v>190</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1">
@@ -7394,7 +7394,7 @@
     </row>
     <row r="125" spans="1:30">
       <c r="A125" s="5" t="s">
-        <v>125</v>
+        <v>191</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1">
@@ -7432,7 +7432,7 @@
     </row>
     <row r="126" spans="1:30">
       <c r="A126" s="5" t="s">
-        <v>126</v>
+        <v>192</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1">
@@ -7470,7 +7470,7 @@
     </row>
     <row r="127" spans="1:30">
       <c r="A127" s="5" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1">
@@ -7508,7 +7508,7 @@
     </row>
     <row r="128" spans="1:30">
       <c r="A128" s="5" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1">
@@ -7546,7 +7546,7 @@
     </row>
     <row r="129" spans="1:30">
       <c r="A129" s="5" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1">
@@ -7590,7 +7590,7 @@
     </row>
     <row r="130" spans="1:30">
       <c r="A130" s="5" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1">
@@ -7634,7 +7634,7 @@
     </row>
     <row r="131" spans="1:30">
       <c r="A131" s="5" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1">
@@ -7678,7 +7678,7 @@
     </row>
     <row r="132" spans="1:30">
       <c r="A132" s="5" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1">
@@ -7724,7 +7724,7 @@
     </row>
     <row r="133" spans="1:30">
       <c r="A133" s="5" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1">
@@ -7770,7 +7770,7 @@
     </row>
     <row r="134" spans="1:30">
       <c r="A134" s="5" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1">
@@ -7816,7 +7816,7 @@
     </row>
     <row r="135" spans="1:30">
       <c r="A135" s="5" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="1">
@@ -7862,7 +7862,7 @@
     </row>
     <row r="136" spans="1:30">
       <c r="A136" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1">
@@ -9142,7 +9142,7 @@
     </row>
     <row r="164" spans="1:30">
       <c r="A164" s="5" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1">
@@ -9194,7 +9194,7 @@
     </row>
     <row r="165" spans="1:30">
       <c r="A165" s="5" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B165" s="5"/>
       <c r="C165" s="1">
@@ -9246,7 +9246,7 @@
     </row>
     <row r="166" spans="1:30">
       <c r="A166" s="5" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B166" s="5"/>
       <c r="C166" s="1">
@@ -9298,7 +9298,7 @@
     </row>
     <row r="167" spans="1:30">
       <c r="A167" s="5" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="B167" s="5"/>
       <c r="C167" s="1">
@@ -9350,7 +9350,7 @@
     </row>
     <row r="168" spans="1:30">
       <c r="A168" s="5" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="B168" s="5"/>
       <c r="C168" s="1">
@@ -9402,7 +9402,7 @@
     </row>
     <row r="169" spans="1:30">
       <c r="A169" s="5" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B169" s="5"/>
       <c r="C169" s="1">
@@ -9454,7 +9454,7 @@
     </row>
     <row r="170" spans="1:30">
       <c r="A170" s="5" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B170" s="5"/>
       <c r="C170" s="1">
@@ -9506,7 +9506,7 @@
     </row>
     <row r="171" spans="1:30">
       <c r="A171" s="5" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B171" s="5"/>
       <c r="C171" s="1">
@@ -9558,7 +9558,7 @@
     </row>
     <row r="172" spans="1:30">
       <c r="A172" s="5" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B172" s="5"/>
       <c r="C172" s="1">
@@ -9610,7 +9610,7 @@
     </row>
     <row r="173" spans="1:30">
       <c r="A173" s="5" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B173" s="5"/>
       <c r="C173" s="1">
@@ -9662,7 +9662,7 @@
     </row>
     <row r="174" spans="1:30">
       <c r="A174" s="5" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B174" s="5"/>
       <c r="C174" s="1">
@@ -9714,7 +9714,7 @@
     </row>
     <row r="175" spans="1:30">
       <c r="A175" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B175" s="5"/>
       <c r="C175" s="1">
@@ -9766,7 +9766,7 @@
     </row>
     <row r="176" spans="1:30">
       <c r="A176" s="5" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="B176" s="5"/>
       <c r="C176" s="1">
@@ -9818,7 +9818,7 @@
     </row>
     <row r="177" spans="1:30">
       <c r="A177" s="5" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B177" s="5"/>
       <c r="C177" s="1">
@@ -9870,7 +9870,7 @@
     </row>
     <row r="178" spans="1:30">
       <c r="A178" s="5" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B178" s="5"/>
       <c r="C178" s="1">
@@ -9922,7 +9922,7 @@
     </row>
     <row r="179" spans="1:30">
       <c r="A179" s="5" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="B179" s="5"/>
       <c r="C179" s="1">
@@ -9974,7 +9974,7 @@
     </row>
     <row r="180" spans="1:30">
       <c r="A180" s="5" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="B180" s="5"/>
       <c r="C180" s="1">
@@ -10026,7 +10026,7 @@
     </row>
     <row r="181" spans="1:30">
       <c r="A181" s="5" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="B181" s="5"/>
       <c r="C181" s="1">
@@ -10078,7 +10078,7 @@
     </row>
     <row r="182" spans="1:30">
       <c r="A182" s="5" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="B182" s="5"/>
       <c r="C182" s="1">
@@ -10130,7 +10130,7 @@
     </row>
     <row r="183" spans="1:30">
       <c r="A183" s="5" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="B183" s="5"/>
       <c r="C183" s="1">
@@ -10182,7 +10182,7 @@
     </row>
     <row r="184" spans="1:30">
       <c r="A184" s="5" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="B184" s="5"/>
       <c r="C184" s="1">
@@ -10234,7 +10234,7 @@
     </row>
     <row r="185" spans="1:30">
       <c r="A185" s="5" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B185" s="5"/>
       <c r="C185" s="1">
@@ -10286,7 +10286,7 @@
     </row>
     <row r="186" spans="1:30">
       <c r="A186" s="5" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B186" s="5"/>
       <c r="C186" s="1">
@@ -10338,7 +10338,7 @@
     </row>
     <row r="187" spans="1:30">
       <c r="A187" s="5" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="B187" s="5"/>
       <c r="C187" s="1">
@@ -10390,7 +10390,7 @@
     </row>
     <row r="188" spans="1:30">
       <c r="A188" s="5" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="B188" s="5"/>
       <c r="C188" s="1">
@@ -10442,7 +10442,7 @@
     </row>
     <row r="189" spans="1:30">
       <c r="A189" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="B189" s="5"/>
       <c r="C189" s="1">
@@ -10494,7 +10494,7 @@
     </row>
     <row r="190" spans="1:30">
       <c r="A190" s="5" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="B190" s="5"/>
       <c r="C190" s="1">
@@ -10546,7 +10546,7 @@
     </row>
     <row r="191" spans="1:30">
       <c r="A191" s="5" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="B191" s="5"/>
       <c r="C191" s="1">
@@ -10598,7 +10598,7 @@
     </row>
     <row r="192" spans="1:30">
       <c r="A192" s="5" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B192" s="5"/>
       <c r="C192" s="1">
@@ -10650,7 +10650,7 @@
     </row>
     <row r="193" spans="1:30">
       <c r="A193" s="5" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="B193" s="5"/>
       <c r="C193" s="1">
@@ -10702,7 +10702,7 @@
     </row>
     <row r="194" spans="1:30">
       <c r="A194" s="5" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="B194" s="5"/>
       <c r="C194" s="1">
@@ -10754,7 +10754,7 @@
     </row>
     <row r="195" spans="1:30">
       <c r="A195" s="5" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="B195" s="5"/>
       <c r="C195" s="1">
@@ -10806,7 +10806,7 @@
     </row>
     <row r="196" spans="1:30">
       <c r="A196" s="5" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="B196" s="5"/>
       <c r="C196" s="1">
@@ -10858,7 +10858,7 @@
     </row>
     <row r="197" spans="1:30">
       <c r="A197" s="5" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B197" s="5"/>
       <c r="C197" s="1">
@@ -10900,7 +10900,7 @@
     </row>
     <row r="198" spans="1:30">
       <c r="A198" s="5" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1">
@@ -10954,7 +10954,7 @@
     </row>
     <row r="199" spans="1:30">
       <c r="A199" s="5" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1">
@@ -11008,7 +11008,7 @@
     </row>
     <row r="200" spans="1:30">
       <c r="A200" s="5" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1">
@@ -11062,7 +11062,7 @@
     </row>
     <row r="201" spans="1:30">
       <c r="A201" s="5" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1">
@@ -11116,7 +11116,7 @@
     </row>
     <row r="202" spans="1:30">
       <c r="A202" s="5" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1">
@@ -11170,7 +11170,7 @@
     </row>
     <row r="203" spans="1:30">
       <c r="A203" s="5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1">
@@ -11224,7 +11224,7 @@
     </row>
     <row r="204" spans="1:30">
       <c r="A204" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1">

</xml_diff>

<commit_message>
update wheat validation to include wongan83 site
</commit_message>
<xml_diff>
--- a/Tests/Wheat/Observed.xlsx
+++ b/Tests/Wheat/Observed.xlsx
@@ -199,36 +199,6 @@
     <t>Wheat_Moora94_N50</t>
   </si>
   <si>
-    <t>Wheat_Wongan83Ripped_RippedN000</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Ripped_RippedN010</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Ripped_RippedN025</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Ripped_RippedN050</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Ripped_RippedN100</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Unripped_UnrippedN000</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Unripped_UnrippedN010</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Unripped_UnrippedN025</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Unripped_UnrippedN050</t>
-  </si>
-  <si>
-    <t>Wheat_Wongan83Unripped_UnrippedN100</t>
-  </si>
-  <si>
     <t>Wheat_Wongan83_Single</t>
   </si>
   <si>
@@ -602,6 +572,36 @@
   </si>
   <si>
     <t>mouseDamageTiller50</t>
+  </si>
+  <si>
+    <t>Wongan83SoilRippedN0</t>
+  </si>
+  <si>
+    <t>Wongan83SoilRippedN10</t>
+  </si>
+  <si>
+    <t>Wongan83SoilRippedN25</t>
+  </si>
+  <si>
+    <t>Wongan83SoilRippedN50</t>
+  </si>
+  <si>
+    <t>Wongan83SoilRippedN100</t>
+  </si>
+  <si>
+    <t>Wongan83SoilUnrippedN0</t>
+  </si>
+  <si>
+    <t>Wongan83SoilUnrippedN10</t>
+  </si>
+  <si>
+    <t>Wongan83SoilUnrippedN25</t>
+  </si>
+  <si>
+    <t>Wongan83SoilUnrippedN50</t>
+  </si>
+  <si>
+    <t>Wongan83SoilUnrippedN100</t>
   </si>
 </sst>
 </file>
@@ -951,9 +951,9 @@
   <dimension ref="A1:AD226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="588" topLeftCell="A111" activePane="bottomLeft"/>
+      <pane ySplit="588" topLeftCell="A208" activePane="bottomLeft"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="B112" sqref="B112:B128"/>
+      <selection pane="bottomLeft" activeCell="A220" sqref="A220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1011,10 +1011,10 @@
         <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>19</v>
@@ -1074,7 +1074,7 @@
         <v>45</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>46</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
@@ -1158,7 +1158,7 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1">
@@ -1196,7 +1196,7 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
@@ -1234,7 +1234,7 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
@@ -1272,7 +1272,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
@@ -1310,7 +1310,7 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="5" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -1348,7 +1348,7 @@
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
@@ -1386,7 +1386,7 @@
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
@@ -1424,7 +1424,7 @@
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
@@ -1462,7 +1462,7 @@
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
@@ -1500,7 +1500,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
@@ -1538,7 +1538,7 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
@@ -1576,7 +1576,7 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1">
@@ -1614,7 +1614,7 @@
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1">
@@ -1652,7 +1652,7 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
@@ -1690,7 +1690,7 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
@@ -1728,7 +1728,7 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
@@ -1766,7 +1766,7 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1">
@@ -1804,7 +1804,7 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
@@ -1842,7 +1842,7 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
@@ -1880,7 +1880,7 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1">
@@ -1918,7 +1918,7 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1">
@@ -1956,7 +1956,7 @@
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1">
@@ -4056,7 +4056,7 @@
     </row>
     <row r="70" spans="1:30">
       <c r="A70" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B70" s="2">
         <v>33797</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="71" spans="1:30">
       <c r="A71" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B71" s="2">
         <v>33812</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="72" spans="1:30">
       <c r="A72" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B72" s="2">
         <v>33840</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="73" spans="1:30">
       <c r="A73" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B73" s="2">
         <v>33856</v>
@@ -4328,7 +4328,7 @@
     </row>
     <row r="74" spans="1:30">
       <c r="A74" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B74" s="2">
         <v>33877</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="75" spans="1:30">
       <c r="A75" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B75" s="2">
         <v>33889</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="76" spans="1:30">
       <c r="A76" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B76" s="2">
         <v>33907</v>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="77" spans="1:30">
       <c r="A77" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B77" s="2">
         <v>33797</v>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="78" spans="1:30">
       <c r="A78" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B78" s="2">
         <v>33812</v>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="79" spans="1:30">
       <c r="A79" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B79" s="2">
         <v>33840</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="80" spans="1:30">
       <c r="A80" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B80" s="2">
         <v>33856</v>
@@ -4804,7 +4804,7 @@
     </row>
     <row r="81" spans="1:30">
       <c r="A81" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B81" s="2">
         <v>33877</v>
@@ -4876,7 +4876,7 @@
     </row>
     <row r="82" spans="1:30">
       <c r="A82" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B82" s="2">
         <v>33889</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="83" spans="1:30">
       <c r="A83" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B83" s="2">
         <v>33907</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="84" spans="1:30">
       <c r="A84" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B84" s="2">
         <v>33797</v>
@@ -5072,7 +5072,7 @@
     </row>
     <row r="85" spans="1:30">
       <c r="A85" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B85" s="2">
         <v>33812</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="86" spans="1:30">
       <c r="A86" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B86" s="2">
         <v>33840</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="87" spans="1:30">
       <c r="A87" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B87" s="2">
         <v>33856</v>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="88" spans="1:30">
       <c r="A88" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B88" s="2">
         <v>33877</v>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="89" spans="1:30">
       <c r="A89" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B89" s="2">
         <v>33889</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="90" spans="1:30">
       <c r="A90" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B90" s="2">
         <v>33907</v>
@@ -5484,7 +5484,7 @@
     </row>
     <row r="91" spans="1:30">
       <c r="A91" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B91" s="2">
         <v>33797</v>
@@ -5548,7 +5548,7 @@
     </row>
     <row r="92" spans="1:30">
       <c r="A92" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B92" s="2">
         <v>33812</v>
@@ -5612,7 +5612,7 @@
     </row>
     <row r="93" spans="1:30">
       <c r="A93" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B93" s="2">
         <v>33840</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="94" spans="1:30">
       <c r="A94" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B94" s="2">
         <v>33856</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="95" spans="1:30">
       <c r="A95" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B95" s="2">
         <v>33877</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="96" spans="1:30">
       <c r="A96" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B96" s="2">
         <v>33889</v>
@@ -5904,7 +5904,7 @@
     </row>
     <row r="97" spans="1:30">
       <c r="A97" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B97" s="2">
         <v>33907</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="98" spans="1:30">
       <c r="A98" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B98" s="2">
         <v>33797</v>
@@ -6024,7 +6024,7 @@
     </row>
     <row r="99" spans="1:30">
       <c r="A99" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B99" s="2">
         <v>33812</v>
@@ -6088,7 +6088,7 @@
     </row>
     <row r="100" spans="1:30">
       <c r="A100" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B100" s="2">
         <v>33840</v>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="101" spans="1:30">
       <c r="A101" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B101" s="2">
         <v>33856</v>
@@ -6232,7 +6232,7 @@
     </row>
     <row r="102" spans="1:30">
       <c r="A102" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B102" s="2">
         <v>33877</v>
@@ -6304,7 +6304,7 @@
     </row>
     <row r="103" spans="1:30">
       <c r="A103" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B103" s="2">
         <v>33889</v>
@@ -6368,7 +6368,7 @@
     </row>
     <row r="104" spans="1:30">
       <c r="A104" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B104" s="2">
         <v>33907</v>
@@ -6424,7 +6424,7 @@
     </row>
     <row r="105" spans="1:30">
       <c r="A105" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B105" s="2">
         <v>33797</v>
@@ -6488,7 +6488,7 @@
     </row>
     <row r="106" spans="1:30">
       <c r="A106" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B106" s="2">
         <v>33812</v>
@@ -6552,7 +6552,7 @@
     </row>
     <row r="107" spans="1:30">
       <c r="A107" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B107" s="2">
         <v>33840</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="108" spans="1:30">
       <c r="A108" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B108" s="2">
         <v>33856</v>
@@ -6696,7 +6696,7 @@
     </row>
     <row r="109" spans="1:30">
       <c r="A109" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B109" s="2">
         <v>33877</v>
@@ -6768,7 +6768,7 @@
     </row>
     <row r="110" spans="1:30">
       <c r="A110" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B110" s="2">
         <v>33889</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="111" spans="1:30">
       <c r="A111" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B111" s="2">
         <v>33907</v>
@@ -6900,7 +6900,7 @@
     </row>
     <row r="112" spans="1:30">
       <c r="A112" s="5" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1">
@@ -6938,7 +6938,7 @@
     </row>
     <row r="113" spans="1:30">
       <c r="A113" s="5" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1">
@@ -6976,7 +6976,7 @@
     </row>
     <row r="114" spans="1:30">
       <c r="A114" s="5" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1">
@@ -7014,7 +7014,7 @@
     </row>
     <row r="115" spans="1:30">
       <c r="A115" s="5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1">
@@ -7052,7 +7052,7 @@
     </row>
     <row r="116" spans="1:30">
       <c r="A116" s="5" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1">
@@ -7090,7 +7090,7 @@
     </row>
     <row r="117" spans="1:30">
       <c r="A117" s="5" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1">
@@ -7128,7 +7128,7 @@
     </row>
     <row r="118" spans="1:30">
       <c r="A118" s="5" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1">
@@ -7166,7 +7166,7 @@
     </row>
     <row r="119" spans="1:30">
       <c r="A119" s="5" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1">
@@ -7204,7 +7204,7 @@
     </row>
     <row r="120" spans="1:30">
       <c r="A120" s="5" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1">
@@ -7242,7 +7242,7 @@
     </row>
     <row r="121" spans="1:30">
       <c r="A121" s="5" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1">
@@ -7280,7 +7280,7 @@
     </row>
     <row r="122" spans="1:30">
       <c r="A122" s="5" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1">
@@ -7318,7 +7318,7 @@
     </row>
     <row r="123" spans="1:30">
       <c r="A123" s="5" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1">
@@ -7356,7 +7356,7 @@
     </row>
     <row r="124" spans="1:30">
       <c r="A124" s="5" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1">
@@ -7394,7 +7394,7 @@
     </row>
     <row r="125" spans="1:30">
       <c r="A125" s="5" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1">
@@ -7432,7 +7432,7 @@
     </row>
     <row r="126" spans="1:30">
       <c r="A126" s="5" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1">
@@ -7470,7 +7470,7 @@
     </row>
     <row r="127" spans="1:30">
       <c r="A127" s="5" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1">
@@ -7508,7 +7508,7 @@
     </row>
     <row r="128" spans="1:30">
       <c r="A128" s="5" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1">
@@ -7546,7 +7546,7 @@
     </row>
     <row r="129" spans="1:30">
       <c r="A129" s="5" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1">
@@ -7590,7 +7590,7 @@
     </row>
     <row r="130" spans="1:30">
       <c r="A130" s="5" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1">
@@ -7634,7 +7634,7 @@
     </row>
     <row r="131" spans="1:30">
       <c r="A131" s="5" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1">
@@ -7678,7 +7678,7 @@
     </row>
     <row r="132" spans="1:30">
       <c r="A132" s="5" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1">
@@ -7724,7 +7724,7 @@
     </row>
     <row r="133" spans="1:30">
       <c r="A133" s="5" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1">
@@ -7770,7 +7770,7 @@
     </row>
     <row r="134" spans="1:30">
       <c r="A134" s="5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1">
@@ -7816,7 +7816,7 @@
     </row>
     <row r="135" spans="1:30">
       <c r="A135" s="5" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="1">
@@ -7862,7 +7862,7 @@
     </row>
     <row r="136" spans="1:30">
       <c r="A136" s="5" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1">
@@ -7908,7 +7908,7 @@
     </row>
     <row r="137" spans="1:30">
       <c r="A137" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1">
@@ -7952,7 +7952,7 @@
     </row>
     <row r="138" spans="1:30">
       <c r="A138" s="5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1">
@@ -7996,7 +7996,7 @@
     </row>
     <row r="139" spans="1:30">
       <c r="A139" s="5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1">
@@ -8040,7 +8040,7 @@
     </row>
     <row r="140" spans="1:30">
       <c r="A140" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1">
@@ -8084,7 +8084,7 @@
     </row>
     <row r="141" spans="1:30">
       <c r="A141" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1">
@@ -8128,7 +8128,7 @@
     </row>
     <row r="142" spans="1:30">
       <c r="A142" s="5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1">
@@ -8172,7 +8172,7 @@
     </row>
     <row r="143" spans="1:30">
       <c r="A143" s="5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1">
@@ -8216,7 +8216,7 @@
     </row>
     <row r="144" spans="1:30">
       <c r="A144" s="5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1">
@@ -8260,7 +8260,7 @@
     </row>
     <row r="145" spans="1:30">
       <c r="A145" s="5" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1">
@@ -8304,7 +8304,7 @@
     </row>
     <row r="146" spans="1:30">
       <c r="A146" s="5" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1">
@@ -8348,7 +8348,7 @@
     </row>
     <row r="147" spans="1:30">
       <c r="A147" s="5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1">
@@ -8392,7 +8392,7 @@
     </row>
     <row r="148" spans="1:30">
       <c r="A148" s="5" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1">
@@ -8436,7 +8436,7 @@
     </row>
     <row r="149" spans="1:30">
       <c r="A149" s="5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1">
@@ -8480,7 +8480,7 @@
     </row>
     <row r="150" spans="1:30">
       <c r="A150" s="5" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1">
@@ -8524,7 +8524,7 @@
     </row>
     <row r="151" spans="1:30">
       <c r="A151" s="5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1">
@@ -8568,7 +8568,7 @@
     </row>
     <row r="152" spans="1:30">
       <c r="A152" s="5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1">
@@ -8878,7 +8878,7 @@
     </row>
     <row r="158" spans="1:30">
       <c r="A158" s="5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1">
@@ -8922,7 +8922,7 @@
     </row>
     <row r="159" spans="1:30">
       <c r="A159" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1">
@@ -8966,7 +8966,7 @@
     </row>
     <row r="160" spans="1:30">
       <c r="A160" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1">
@@ -9010,7 +9010,7 @@
     </row>
     <row r="161" spans="1:30">
       <c r="A161" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B161" s="1"/>
       <c r="C161" s="1">
@@ -9054,7 +9054,7 @@
     </row>
     <row r="162" spans="1:30">
       <c r="A162" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1">
@@ -9098,7 +9098,7 @@
     </row>
     <row r="163" spans="1:30">
       <c r="A163" s="5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B163" s="1"/>
       <c r="C163" s="1">
@@ -9142,7 +9142,7 @@
     </row>
     <row r="164" spans="1:30">
       <c r="A164" s="5" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1">
@@ -9194,7 +9194,7 @@
     </row>
     <row r="165" spans="1:30">
       <c r="A165" s="5" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B165" s="5"/>
       <c r="C165" s="1">
@@ -9246,7 +9246,7 @@
     </row>
     <row r="166" spans="1:30">
       <c r="A166" s="5" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B166" s="5"/>
       <c r="C166" s="1">
@@ -9298,7 +9298,7 @@
     </row>
     <row r="167" spans="1:30">
       <c r="A167" s="5" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B167" s="5"/>
       <c r="C167" s="1">
@@ -9350,7 +9350,7 @@
     </row>
     <row r="168" spans="1:30">
       <c r="A168" s="5" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B168" s="5"/>
       <c r="C168" s="1">
@@ -9402,7 +9402,7 @@
     </row>
     <row r="169" spans="1:30">
       <c r="A169" s="5" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B169" s="5"/>
       <c r="C169" s="1">
@@ -9454,7 +9454,7 @@
     </row>
     <row r="170" spans="1:30">
       <c r="A170" s="5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B170" s="5"/>
       <c r="C170" s="1">
@@ -9506,7 +9506,7 @@
     </row>
     <row r="171" spans="1:30">
       <c r="A171" s="5" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B171" s="5"/>
       <c r="C171" s="1">
@@ -9558,7 +9558,7 @@
     </row>
     <row r="172" spans="1:30">
       <c r="A172" s="5" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B172" s="5"/>
       <c r="C172" s="1">
@@ -9610,7 +9610,7 @@
     </row>
     <row r="173" spans="1:30">
       <c r="A173" s="5" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B173" s="5"/>
       <c r="C173" s="1">
@@ -9662,7 +9662,7 @@
     </row>
     <row r="174" spans="1:30">
       <c r="A174" s="5" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B174" s="5"/>
       <c r="C174" s="1">
@@ -9714,7 +9714,7 @@
     </row>
     <row r="175" spans="1:30">
       <c r="A175" s="5" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B175" s="5"/>
       <c r="C175" s="1">
@@ -9766,7 +9766,7 @@
     </row>
     <row r="176" spans="1:30">
       <c r="A176" s="5" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B176" s="5"/>
       <c r="C176" s="1">
@@ -9818,7 +9818,7 @@
     </row>
     <row r="177" spans="1:30">
       <c r="A177" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B177" s="5"/>
       <c r="C177" s="1">
@@ -9870,7 +9870,7 @@
     </row>
     <row r="178" spans="1:30">
       <c r="A178" s="5" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B178" s="5"/>
       <c r="C178" s="1">
@@ -9922,7 +9922,7 @@
     </row>
     <row r="179" spans="1:30">
       <c r="A179" s="5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B179" s="5"/>
       <c r="C179" s="1">
@@ -9974,7 +9974,7 @@
     </row>
     <row r="180" spans="1:30">
       <c r="A180" s="5" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B180" s="5"/>
       <c r="C180" s="1">
@@ -10026,7 +10026,7 @@
     </row>
     <row r="181" spans="1:30">
       <c r="A181" s="5" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B181" s="5"/>
       <c r="C181" s="1">
@@ -10078,7 +10078,7 @@
     </row>
     <row r="182" spans="1:30">
       <c r="A182" s="5" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B182" s="5"/>
       <c r="C182" s="1">
@@ -10130,7 +10130,7 @@
     </row>
     <row r="183" spans="1:30">
       <c r="A183" s="5" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B183" s="5"/>
       <c r="C183" s="1">
@@ -10182,7 +10182,7 @@
     </row>
     <row r="184" spans="1:30">
       <c r="A184" s="5" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B184" s="5"/>
       <c r="C184" s="1">
@@ -10234,7 +10234,7 @@
     </row>
     <row r="185" spans="1:30">
       <c r="A185" s="5" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B185" s="5"/>
       <c r="C185" s="1">
@@ -10286,7 +10286,7 @@
     </row>
     <row r="186" spans="1:30">
       <c r="A186" s="5" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B186" s="5"/>
       <c r="C186" s="1">
@@ -10338,7 +10338,7 @@
     </row>
     <row r="187" spans="1:30">
       <c r="A187" s="5" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B187" s="5"/>
       <c r="C187" s="1">
@@ -10390,7 +10390,7 @@
     </row>
     <row r="188" spans="1:30">
       <c r="A188" s="5" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B188" s="5"/>
       <c r="C188" s="1">
@@ -10442,7 +10442,7 @@
     </row>
     <row r="189" spans="1:30">
       <c r="A189" s="5" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B189" s="5"/>
       <c r="C189" s="1">
@@ -10494,7 +10494,7 @@
     </row>
     <row r="190" spans="1:30">
       <c r="A190" s="5" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B190" s="5"/>
       <c r="C190" s="1">
@@ -10546,7 +10546,7 @@
     </row>
     <row r="191" spans="1:30">
       <c r="A191" s="5" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B191" s="5"/>
       <c r="C191" s="1">
@@ -10598,7 +10598,7 @@
     </row>
     <row r="192" spans="1:30">
       <c r="A192" s="5" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B192" s="5"/>
       <c r="C192" s="1">
@@ -10650,7 +10650,7 @@
     </row>
     <row r="193" spans="1:30">
       <c r="A193" s="5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B193" s="5"/>
       <c r="C193" s="1">
@@ -10702,7 +10702,7 @@
     </row>
     <row r="194" spans="1:30">
       <c r="A194" s="5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B194" s="5"/>
       <c r="C194" s="1">
@@ -10754,7 +10754,7 @@
     </row>
     <row r="195" spans="1:30">
       <c r="A195" s="5" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B195" s="5"/>
       <c r="C195" s="1">
@@ -10806,7 +10806,7 @@
     </row>
     <row r="196" spans="1:30">
       <c r="A196" s="5" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B196" s="5"/>
       <c r="C196" s="1">
@@ -10858,7 +10858,7 @@
     </row>
     <row r="197" spans="1:30">
       <c r="A197" s="5" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B197" s="5"/>
       <c r="C197" s="1">
@@ -10900,7 +10900,7 @@
     </row>
     <row r="198" spans="1:30">
       <c r="A198" s="5" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1">
@@ -10954,7 +10954,7 @@
     </row>
     <row r="199" spans="1:30">
       <c r="A199" s="5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1">
@@ -11008,7 +11008,7 @@
     </row>
     <row r="200" spans="1:30">
       <c r="A200" s="5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1">
@@ -11062,7 +11062,7 @@
     </row>
     <row r="201" spans="1:30">
       <c r="A201" s="5" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1">
@@ -11116,7 +11116,7 @@
     </row>
     <row r="202" spans="1:30">
       <c r="A202" s="5" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1">
@@ -11170,7 +11170,7 @@
     </row>
     <row r="203" spans="1:30">
       <c r="A203" s="5" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1">
@@ -11224,7 +11224,7 @@
     </row>
     <row r="204" spans="1:30">
       <c r="A204" s="5" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1">
@@ -11474,7 +11474,7 @@
     </row>
     <row r="209" spans="1:30">
       <c r="A209" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1">
@@ -11518,7 +11518,7 @@
     </row>
     <row r="210" spans="1:30">
       <c r="A210" s="5" t="s">
-        <v>60</v>
+        <v>185</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1">
@@ -11570,7 +11570,7 @@
     </row>
     <row r="211" spans="1:30">
       <c r="A211" s="5" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1">
@@ -11622,7 +11622,7 @@
     </row>
     <row r="212" spans="1:30">
       <c r="A212" s="5" t="s">
-        <v>62</v>
+        <v>187</v>
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1">
@@ -11674,7 +11674,7 @@
     </row>
     <row r="213" spans="1:30">
       <c r="A213" s="5" t="s">
-        <v>63</v>
+        <v>188</v>
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1">
@@ -11726,7 +11726,7 @@
     </row>
     <row r="214" spans="1:30">
       <c r="A214" s="5" t="s">
-        <v>64</v>
+        <v>189</v>
       </c>
       <c r="B214" s="1"/>
       <c r="C214" s="1">
@@ -11778,7 +11778,7 @@
     </row>
     <row r="215" spans="1:30">
       <c r="A215" s="5" t="s">
-        <v>65</v>
+        <v>190</v>
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1">
@@ -11830,7 +11830,7 @@
     </row>
     <row r="216" spans="1:30">
       <c r="A216" s="5" t="s">
-        <v>66</v>
+        <v>191</v>
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1">
@@ -11882,7 +11882,7 @@
     </row>
     <row r="217" spans="1:30">
       <c r="A217" s="5" t="s">
-        <v>67</v>
+        <v>192</v>
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1">
@@ -11934,7 +11934,7 @@
     </row>
     <row r="218" spans="1:30">
       <c r="A218" s="5" t="s">
-        <v>68</v>
+        <v>193</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1">
@@ -11986,7 +11986,7 @@
     </row>
     <row r="219" spans="1:30">
       <c r="A219" s="5" t="s">
-        <v>69</v>
+        <v>194</v>
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1">
@@ -12238,7 +12238,7 @@
     </row>
     <row r="224" spans="1:30">
       <c r="A224" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1">
@@ -12278,7 +12278,7 @@
     </row>
     <row r="225" spans="1:30">
       <c r="A225" s="5" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B225" s="1"/>
       <c r="C225" s="1">
@@ -12318,7 +12318,7 @@
     </row>
     <row r="226" spans="1:30">
       <c r="A226" s="5" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B226" s="1"/>
       <c r="C226" s="1">

</xml_diff>